<commit_message>
:construction: MultipleSheetExcelGenerator 인자 순서 변경
</commit_message>
<xml_diff>
--- a/src/test/resources/test_multiple.xlsx
+++ b/src/test/resources/test_multiple.xlsx
@@ -272,13 +272,13 @@
         </is>
       </c>
       <c r="C2" s="5" t="n">
-        <v>975502.0</v>
+        <v>889182.0</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>815115.3125</v>
+        <v>914770.75</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>361097.0</v>
+        <v>188138.0</v>
       </c>
     </row>
     <row r="3">
@@ -293,13 +293,13 @@
         </is>
       </c>
       <c r="C3" s="5" t="n">
-        <v>784445.0</v>
+        <v>203702.0</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>514558.3125</v>
+        <v>754265.3125</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>262936.0</v>
+        <v>861124.0</v>
       </c>
     </row>
   </sheetData>
@@ -354,13 +354,13 @@
         </is>
       </c>
       <c r="C2" s="5" t="n">
-        <v>47382.0</v>
+        <v>270245.0</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>381.4101257324219</v>
+        <v>533421.75</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>354392.0</v>
+        <v>123410.0</v>
       </c>
     </row>
     <row r="3">
@@ -375,13 +375,13 @@
         </is>
       </c>
       <c r="C3" s="5" t="n">
-        <v>769894.0</v>
+        <v>851954.0</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>193235.515625</v>
+        <v>344267.78125</v>
       </c>
       <c r="E3" s="7" t="n">
-        <v>90824.0</v>
+        <v>298359.0</v>
       </c>
     </row>
   </sheetData>
@@ -440,13 +440,13 @@
         </is>
       </c>
       <c r="C2" s="5" t="n">
-        <v>582381.0</v>
+        <v>222746.0</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>368285.96875</v>
+        <v>116392.609375</v>
       </c>
       <c r="E2" s="7" t="n">
-        <v>8332.0</v>
+        <v>347667.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>